<commit_message>
BSTATS-105: All teams in season upload for one league (just teams not players)
</commit_message>
<xml_diff>
--- a/leagues_NL_1961_teams.xlsx
+++ b/leagues_NL_1961_teams.xlsx
@@ -3,23 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev-tools\github\bbstats\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27600" windowHeight="10320"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17385" windowHeight="6465"/>
   </bookViews>
   <sheets>
     <sheet name="leagues_NL_1961_expanded_standi" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
   <si>
     <t>CHC</t>
   </si>
@@ -139,6 +135,9 @@
   </si>
   <si>
     <t>Missouri</t>
+  </si>
+  <si>
+    <t>Abbreviation</t>
   </si>
 </sst>
 </file>
@@ -952,11 +951,12 @@
   <dimension ref="A2:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="22.28515625" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
     <col min="5" max="5" width="18.28515625" customWidth="1"/>
@@ -965,6 +965,9 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>

</xml_diff>